<commit_message>
implementation of oak and fuzzywuzzy
</commit_message>
<xml_diff>
--- a/more_grounding/evaluation_summary_post_ontoGPT_df.xlsx
+++ b/more_grounding/evaluation_summary_post_ontoGPT_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niyone/Desktop/maxo/automaxo/more_grounding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBB606E-D86D-F84C-AF89-3335819D6AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546BBD8D-2FC8-E843-A129-703D0B6A8EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2204,7 +2204,7 @@
   <dimension ref="A1:O235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>